<commit_message>
Updated some resistor values
</commit_message>
<xml_diff>
--- a/Transistor_Ladder_VCF/PCB/Transistor_Ladder_VCF_v1_2_1BOM.xlsx
+++ b/Transistor_Ladder_VCF/PCB/Transistor_Ladder_VCF_v1_2_1BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenz Neumann\Documents\Eurorack\Transistor_Ladder_VCF\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2FA903-48BD-4F2B-9F4A-A189B2777523}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F7637B-F14C-4A2A-9B8E-C056B1078C05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,12 +453,6 @@
     <t>RV4,RV6</t>
   </si>
   <si>
-    <t>R3,R9,R16,R25,R27,R29,R31,R48,R61</t>
-  </si>
-  <si>
-    <t>R20,R26,R44,R45,R50,R51,R53,R54,R55,R58,R60</t>
-  </si>
-  <si>
     <t>R1,R2,R4,R10,R12,R14,R18,R19,R28,R34,R39,R40,R41,R56,</t>
   </si>
   <si>
@@ -505,6 +499,12 @@
   </si>
   <si>
     <t>B100k ist working fine ass well, your choice</t>
+  </si>
+  <si>
+    <t>R3,R9,R16,R25,R26,R27,R29,R31,R48,R61</t>
+  </si>
+  <si>
+    <t>R20,R44,R45,R50,R51,R53,R54,R55,R58,R60</t>
   </si>
 </sst>
 </file>
@@ -1674,8 +1674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1717,13 +1717,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C3" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
@@ -1736,13 +1736,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C4" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>16</v>
@@ -1795,7 +1795,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>46</v>
@@ -1814,7 +1814,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>46</v>
@@ -1852,7 +1852,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>46</v>
@@ -1928,7 +1928,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>46</v>
@@ -1947,7 +1947,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>46</v>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>46</v>
@@ -2028,7 +2028,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>9</v>
@@ -2047,7 +2047,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>9</v>
@@ -2134,7 +2134,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>51</v>
@@ -2168,7 +2168,7 @@
         <v>104</v>
       </c>
       <c r="F28" s="22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G28" s="3"/>
     </row>
@@ -2293,7 +2293,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>52</v>
@@ -2370,7 +2370,7 @@
         <v>32</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G40" s="3"/>
     </row>
@@ -2438,7 +2438,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>129</v>
@@ -2705,14 +2705,14 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F71" s="26"/>
       <c r="G71" s="3"/>
     </row>
     <row r="72" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B72" s="13"/>
       <c r="C72" s="14"/>
@@ -2731,7 +2731,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B74" s="8"/>
       <c r="C74" s="9"/>

</xml_diff>

<commit_message>
Updated schematics and BOM
</commit_message>
<xml_diff>
--- a/Transistor_Ladder_VCF/PCB/Transistor_Ladder_VCF_v1_2_1BOM.xlsx
+++ b/Transistor_Ladder_VCF/PCB/Transistor_Ladder_VCF_v1_2_1BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenz Neumann\Documents\Eurorack\Transistor_Ladder_VCF\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBA0D68-031D-419C-903B-0B777879F806}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03675219-6F95-4BF8-8555-B3215384FE42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="165">
   <si>
     <t>Thonkicon</t>
   </si>
@@ -162,9 +162,6 @@
     <t xml:space="preserve">603-RC0603FR-0710KL </t>
   </si>
   <si>
-    <t xml:space="preserve">603-RC0603FR-071K2L </t>
-  </si>
-  <si>
     <t xml:space="preserve">603-RC0603FR-071KL </t>
   </si>
   <si>
@@ -276,18 +273,9 @@
     <t xml:space="preserve">81-PV36W104C01B00 </t>
   </si>
   <si>
-    <t>1V/oct Tuning: Let the Filter self-oscillate, insert a 1V/oct signal and try to calibrate as good as possible. (matching octaves is the easiest way for me)</t>
-  </si>
-  <si>
-    <t>Note: Although this filter can be tuned to 1V/oct, don't expect stable tuning.</t>
-  </si>
-  <si>
     <t>Support and feedback: lorenz-neumann@gmx.de</t>
   </si>
   <si>
-    <t>Adjust the max resonace/self-oscillation level with Q1-Trim for 24dB and  Q2-Trim for 6/13/18dB</t>
-  </si>
-  <si>
     <t>29k4</t>
   </si>
   <si>
@@ -354,9 +342,6 @@
     <t>512-1N4148WS</t>
   </si>
   <si>
-    <t>R43,R57</t>
-  </si>
-  <si>
     <t>R59</t>
   </si>
   <si>
@@ -366,9 +351,6 @@
     <t>RV11</t>
   </si>
   <si>
-    <t>RV9</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -393,9 +375,6 @@
     <t>Set dB/OCT to 24</t>
   </si>
   <si>
-    <t>Set the Cutoff at 12 o'clock. Set Q to max. Adjust "Q Level" (RV10) until there is stable selfoszilation. Check hole Cutoffrange, if nesseary.</t>
-  </si>
-  <si>
     <t>Adjust "Freq. Offset" and "Freq. Tune"(Determinens the Range of the the cutoff-potentiometer.) until the filter can  be closed and opened fully by the Frequency potentiometer.</t>
   </si>
   <si>
@@ -411,9 +390,6 @@
     <t>Troubleshooting:</t>
   </si>
   <si>
-    <t>Check all Solderjoints for bridges, bad soldering ect.</t>
-  </si>
-  <si>
     <t>D8</t>
   </si>
   <si>
@@ -471,9 +447,6 @@
     <t>U2,U3,U5</t>
   </si>
   <si>
-    <t>RV10,RV12</t>
-  </si>
-  <si>
     <t>D3,D4,D5,D6,D7</t>
   </si>
   <si>
@@ -517,6 +490,42 @@
   </si>
   <si>
     <t>Small! Be sure to have some SMD practice! (pitch = 0.95mm)</t>
+  </si>
+  <si>
+    <t>R57</t>
+  </si>
+  <si>
+    <t>R43</t>
+  </si>
+  <si>
+    <t>2K7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">603-RC0603FR-072K2L </t>
+  </si>
+  <si>
+    <t xml:space="preserve">603-RC0603FR-072K7L </t>
+  </si>
+  <si>
+    <t>RV10</t>
+  </si>
+  <si>
+    <t>RV9,RV12</t>
+  </si>
+  <si>
+    <t>Set the Cutoff at 12 o'clock. Set Q to max. Adjust "Q Level" (RV10) until there is stable selfoszilation. Check hole Cutoff-Range, if nesseary.</t>
+  </si>
+  <si>
+    <t>Adjust the max resonace/self-oscillation level with "Q Level" (RV10)</t>
+  </si>
+  <si>
+    <t>1V/Oct Tuning: Let the Filter self-oscillate, insert a 1V/Oct signal and try to calibrate as good as possible. (matching octaves is the easiest way for me)</t>
+  </si>
+  <si>
+    <t>Note: Although this filter can be tuned to 1V/Oct, don't expect temperature-stable tuning.</t>
+  </si>
+  <si>
+    <t>Check all solderjoints for bridges, bad soldering ect.</t>
   </si>
 </sst>
 </file>
@@ -873,7 +882,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1073,21 +1082,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1241,6 +1235,77 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1289,7 +1354,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1300,34 +1365,36 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="17" xfId="42" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="17" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="18" xfId="42" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="18" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1684,10 +1751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1701,38 +1768,42 @@
     <col min="7" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="32" t="s">
+      <c r="D1" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="33" t="s">
-        <v>77</v>
+      <c r="F1" s="37" t="s">
+        <v>76</v>
       </c>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="F2" s="34"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1">
         <v>10</v>
@@ -1748,10 +1819,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1">
         <v>10</v>
@@ -1763,54 +1834,54 @@
         <v>41</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -1826,10 +1897,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="1">
         <v>14</v>
@@ -1845,29 +1916,29 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1">
         <v>5</v>
@@ -1876,190 +1947,190 @@
         <v>18</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>107</v>
+        <v>154</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>72</v>
+        <v>155</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>43</v>
+        <v>157</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>87</v>
+        <v>153</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>100</v>
+        <v>71</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>156</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>132</v>
+        <v>83</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>44</v>
+        <v>84</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>96</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
+      <c r="A16" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="1">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="F16" s="11"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="1">
-        <v>11</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="A17" s="20"/>
       <c r="F17" s="11"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>143</v>
+        <v>25</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" t="s">
-        <v>156</v>
+        <v>7</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>9</v>
@@ -2068,717 +2139,736 @@
         <v>2</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" t="s">
-        <v>155</v>
+        <v>5</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>147</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="C22" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
+      </c>
+      <c r="E22" t="s">
+        <v>146</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="10"/>
+      <c r="A23" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="1">
+        <v>4</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="F23" s="11"/>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="1">
-        <v>2</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A24" s="10"/>
       <c r="F24" s="11"/>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
-        <v>127</v>
+      <c r="A25" s="20" t="s">
+        <v>11</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>104</v>
+        <v>12</v>
       </c>
       <c r="C25" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>106</v>
+        <v>34</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="10"/>
-      <c r="E26" s="21"/>
+      <c r="A26" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>102</v>
+      </c>
       <c r="F26" s="11"/>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="1">
-        <v>3</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F27" s="19"/>
+      <c r="A27" s="10"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="11"/>
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>51</v>
+        <v>137</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="C28" s="1">
-        <v>1</v>
-      </c>
-      <c r="D28" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="E28" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="F28" s="22" t="s">
-        <v>150</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="19"/>
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="F29" s="19"/>
+        <v>99</v>
+      </c>
+      <c r="F29" s="22" t="s">
+        <v>141</v>
+      </c>
       <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F30" s="19"/>
       <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>67</v>
+        <v>90</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>88</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F31" s="11"/>
+      <c r="D31" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="F31" s="19"/>
       <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>67</v>
+        <v>121</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F32" s="11"/>
       <c r="G32" s="3"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>47</v>
+        <v>122</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" s="11"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="1">
         <v>5</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F33" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="10"/>
-      <c r="F34" s="11"/>
+      <c r="F34" s="11" t="s">
+        <v>152</v>
+      </c>
       <c r="G34" s="3"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C35" s="1">
-        <v>1</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E35" s="21" t="s">
-        <v>80</v>
-      </c>
+      <c r="A35" s="10"/>
       <c r="F35" s="11"/>
       <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36" s="1">
         <v>2</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>31</v>
+        <v>4</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>79</v>
       </c>
       <c r="F36" s="11"/>
       <c r="G36" s="3"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
-        <v>110</v>
+        <v>158</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F37" s="11"/>
       <c r="G37" s="3"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="10"/>
+      <c r="A38" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="F38" s="11"/>
       <c r="G38" s="3"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C39" s="1">
-        <v>2</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="A39" s="10"/>
       <c r="F39" s="11"/>
       <c r="G39" s="3"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C40" s="1">
         <v>2</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F40" s="11" t="s">
-        <v>159</v>
-      </c>
+      <c r="F40" s="11"/>
       <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
-        <v>22</v>
+        <v>128</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="1">
+        <v>2</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="C41" s="1">
-        <v>1</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F41" s="11"/>
+      <c r="F41" s="11" t="s">
+        <v>150</v>
+      </c>
       <c r="G41" s="3"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
-        <v>135</v>
+        <v>22</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C42" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="F42" s="11"/>
       <c r="G42" s="3"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C43" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F43" s="11"/>
       <c r="G43" s="3"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="10"/>
+      <c r="A44" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="F44" s="11"/>
       <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C45" s="1">
-        <v>5</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E45" t="s">
-        <v>158</v>
-      </c>
+      <c r="A45" s="10"/>
       <c r="F45" s="11"/>
       <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="C46" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>38</v>
+        <v>120</v>
+      </c>
+      <c r="E46" t="s">
+        <v>149</v>
       </c>
       <c r="F46" s="11"/>
       <c r="G46" s="3"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="35" t="s">
-        <v>115</v>
+      <c r="A47" s="10" t="s">
+        <v>110</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C47" s="1">
+        <v>7</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>96</v>
+      <c r="E47" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="F47" s="11"/>
       <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="35" t="s">
-        <v>117</v>
+      <c r="A48" s="30" t="s">
+        <v>109</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F48" s="11"/>
+      <c r="G48" s="3"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C49" s="1">
         <v>3</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F48" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="G48" s="3"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="35"/>
-      <c r="F49" s="11"/>
+      <c r="F49" s="11" t="s">
+        <v>151</v>
+      </c>
       <c r="G49" s="3"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C50" s="1">
-        <v>3</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>160</v>
-      </c>
+      <c r="A50" s="30"/>
+      <c r="F50" s="11"/>
       <c r="G50" s="3"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51" s="1">
+        <v>3</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F51" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G51" s="3"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="E52" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F52" s="11"/>
+      <c r="G52" s="3"/>
+    </row>
+    <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C51" s="1">
-        <v>1</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F51" s="11"/>
-      <c r="G51" s="3"/>
-    </row>
-    <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B52" s="13" t="s">
+      <c r="C53" s="14">
+        <v>2</v>
+      </c>
+      <c r="D53" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C52" s="14">
-        <v>2</v>
-      </c>
-      <c r="D52" s="14" t="s">
+      <c r="E53" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="E52" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="F52" s="15"/>
-      <c r="G52" s="3"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="6"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
-    </row>
-    <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="16"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="4"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="B55" s="8"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="3"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="3"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="6"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+    </row>
+    <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="16"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="4"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="10"/>
-      <c r="F56" s="26"/>
+      <c r="A56" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="B56" s="8"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="25"/>
       <c r="G56" s="3"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="10" t="s">
-        <v>122</v>
-      </c>
+      <c r="A57" s="10"/>
       <c r="F57" s="26"/>
       <c r="G57" s="3"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="27" t="s">
-        <v>124</v>
+      <c r="A58" s="10" t="s">
+        <v>115</v>
       </c>
       <c r="F58" s="26"/>
       <c r="G58" s="3"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="10" t="s">
-        <v>119</v>
+      <c r="A59" s="27" t="s">
+        <v>117</v>
       </c>
       <c r="F59" s="26"/>
       <c r="G59" s="3"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F60" s="26"/>
       <c r="G60" s="3"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
-        <v>121</v>
+        <v>160</v>
       </c>
       <c r="F61" s="26"/>
       <c r="G61" s="3"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="F62" s="26"/>
       <c r="G62" s="3"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="F63" s="26"/>
       <c r="G63" s="3"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
-        <v>81</v>
+        <v>161</v>
       </c>
       <c r="F64" s="26"/>
       <c r="G64" s="3"/>
     </row>
-    <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="B65" s="13"/>
-      <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="28"/>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="F65" s="26"/>
       <c r="G65" s="3"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="6"/>
-      <c r="B66" s="7"/>
-      <c r="C66" s="6"/>
-      <c r="D66" s="6"/>
-      <c r="E66" s="6"/>
-      <c r="F66" s="23"/>
-    </row>
-    <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="4"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="24"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="B68" s="8"/>
-      <c r="C68" s="9"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="25"/>
-      <c r="G68" s="3"/>
+    <row r="66" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="B66" s="13"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="28"/>
+      <c r="G66" s="3"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" s="6"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="23"/>
+    </row>
+    <row r="68" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="4"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="24"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="10"/>
-      <c r="F69" s="26"/>
+      <c r="A69" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="B69" s="8"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="25"/>
       <c r="G69" s="3"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="10" t="s">
-        <v>126</v>
-      </c>
+      <c r="A70" s="10"/>
       <c r="F70" s="26"/>
       <c r="G70" s="3"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="10" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="F71" s="26"/>
       <c r="G71" s="3"/>
     </row>
-    <row r="72" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="B72" s="13"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="28"/>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F72" s="26"/>
       <c r="G72" s="3"/>
     </row>
     <row r="73" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="16"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="16"/>
-      <c r="D73" s="16"/>
-      <c r="E73" s="16"/>
-      <c r="F73" s="29"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="B74" s="8"/>
-      <c r="C74" s="9"/>
-      <c r="D74" s="9"/>
-      <c r="E74" s="9"/>
-      <c r="F74" s="25"/>
-      <c r="G74" s="3"/>
-    </row>
-    <row r="75" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B75" s="13"/>
-      <c r="C75" s="14"/>
-      <c r="D75" s="14"/>
-      <c r="E75" s="14"/>
-      <c r="F75" s="28"/>
+      <c r="A73" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B73" s="13"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="28"/>
+      <c r="G73" s="3"/>
+    </row>
+    <row r="74" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="16"/>
+      <c r="B74" s="17"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="16"/>
+      <c r="F74" s="29"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="B75" s="8"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="25"/>
       <c r="G75" s="3"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" s="6"/>
-      <c r="B76" s="7"/>
-      <c r="C76" s="6"/>
-      <c r="D76" s="6"/>
-      <c r="E76" s="6"/>
-      <c r="F76" s="6"/>
+    <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B76" s="13"/>
+      <c r="C76" s="14"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="28"/>
+      <c r="G76" s="3"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" s="6"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>